<commit_message>
new generation script using openpyxl
</commit_message>
<xml_diff>
--- a/templates/template_spreadsheet.xlsx
+++ b/templates/template_spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abrown41/PeerMark/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abrown41/progs/PeerMark/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4471EF6-974A-C247-ACC9-5EB61DB038B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773F4B01-1C0D-E444-8C37-D4D7D6037E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="1820" windowWidth="23880" windowHeight="16180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Attendance at group meetings</t>
   </si>
@@ -62,16 +64,16 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">TEAM: </t>
-  </si>
-  <si>
     <t>FINAL SCORE:</t>
   </si>
   <si>
     <t>TOTAL points left:</t>
   </si>
   <si>
-    <t>INPUT total score:</t>
+    <t>Add the information for each team member in the correct column
+Score each aspect for each member of your group (including yourself) between 0 (extremely poor) and 5 (outstanding)
+Scores and comments will be anonymised, so try to give useful (constructive) feedback where possible: that will make this exercise valuable to everyone.  Don't try to format the comments or insert text boxes, simply type the comments in to the cell, and don't worry about how they are rendered.
+You then need to award a final score for each member. You have a maximum total number of marks to give out,  which you can spread out as you wish amongst the team members, but again, with a minimum of 0 and a maximum of 5 for each member. You don't have to allocate all the marks if you don't feel it is warranted, but if you exceed the total then no marks will be allocated.</t>
   </si>
 </sst>
 </file>
@@ -134,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -154,10 +156,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -174,145 +179,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>292100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9588500" y="203200"/>
-          <a:ext cx="3987800" cy="3695700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200"/>
-            <a:t>Instructions will</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0"/>
-            <a:t> go here: you can add them in the instructions file, instructions.txt.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0"/>
-            <a:t>The text here does not appear in the final version. Only the instructions from instructions.txt</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -578,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -592,130 +458,156 @@
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="G2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="113" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" ht="113" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
         <v>10</v>
       </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13">
+      <c r="G11">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="wrong format" error="Please assign a valid score: a whole number between 0 and 5" sqref="B3:E8" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <mergeCells count="1">
+    <mergeCell ref="G2:K9"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="wrong format" error="Please assign a valid score: a whole number between 0 and 5" sqref="B2:E7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Please input a valid score: a whole number between 0 and 5. Total score may not exceed 14 for the team." sqref="E12" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>AND( (SUM($B$12:$E$12)&lt;=14), (SUM($B$12:$E$12) &gt;=0),$E$12=INT($E$12),$E$12&lt;=5)</formula1>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="You can allocate a maximum of 13 points to your team" sqref="G11" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>0</formula1>
+      <formula2>13</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="You can allocate a maximum of 14 points to your team" sqref="G13" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>0</formula1>
-      <formula2>14</formula2>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Please input a valid score: a whole number between 0 and 5. Total score may not exceed 14 for the team." sqref="B12" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>AND( (SUM($B$12:$E$12)&lt;=14), (SUM($B$12:$E$12) &gt;=0),$B$12=INT($B$12),$B$12&lt;=5)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Please input a valid score: a whole number between 0 and 5. Total score may not exceed 14 for the team." sqref="C12" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>AND( (SUM($B$12:$E$12)&lt;=14), (SUM($B$12:$E$12) &gt;=0),$C$12=INT($C$12),$C$12&lt;=5)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Error" error="Please input a valid score: a whole number between 0 and 5. Total score may not exceed 14 for the team." sqref="D12" xr:uid="{00000000-0002-0000-0000-000005000000}">
-      <formula1>AND( (SUM($B$12:$E$12)&lt;=14), (SUM($B$12:$E$12) &gt;=0),$D$12=INT($D$12),$D$12&lt;=5)</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The FINAL SCORE for a team member must be a whole number between 0 and 5, and the TOTAL score for the team cannot exceed 13. " sqref="B11:E11" xr:uid="{DDAA1F25-9543-ED44-A7A2-F609DE9CEDEB}">
+      <formula1>AND(MOD(B$11,1)=0, B$11&lt;=5, B11&gt;=0, SUM($B$11:$E$11) &lt;= $G$11)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>